<commit_message>
Fix indigenous mortality targets.  (Again must be right now)
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_mortality_uploader/indigenous_mortality.xlsx
+++ b/dashboard_loader/indigenous_mortality_uploader/indigenous_mortality.xlsx
@@ -129,11 +129,12 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,12 +153,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -223,7 +218,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,23 +235,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -268,7 +259,7 @@
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2 2 3_Data supply March 23 2012_HPF Delivery 4" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -340,15 +331,15 @@
   </sheetPr>
   <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H109" activeCellId="0" sqref="H109"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C146" activeCellId="0" sqref="C146:G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -383,7 +374,7 @@
       <c r="A3" s="3" t="n">
         <v>1998</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="n">
@@ -406,7 +397,7 @@
       <c r="A4" s="3" t="n">
         <v>1998</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="1" t="n">
@@ -421,7 +412,7 @@
       <c r="F4" s="1" t="n">
         <v>791.8264146</v>
       </c>
-      <c r="G4" s="4" t="n">
+      <c r="G4" s="1" t="n">
         <v>700</v>
       </c>
     </row>
@@ -429,7 +420,7 @@
       <c r="A5" s="3" t="n">
         <v>1998</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1" t="n">
@@ -452,7 +443,7 @@
       <c r="A6" s="3" t="n">
         <v>1998</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="1" t="n">
@@ -475,7 +466,7 @@
       <c r="A7" s="3" t="n">
         <v>1999</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1" t="n">
@@ -498,7 +489,7 @@
       <c r="A8" s="3" t="n">
         <v>1999</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="1" t="n">
@@ -521,7 +512,7 @@
       <c r="A9" s="3" t="n">
         <v>1999</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1" t="n">
@@ -544,7 +535,7 @@
       <c r="A10" s="3" t="n">
         <v>1999</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="n">
@@ -567,7 +558,7 @@
       <c r="A11" s="3" t="n">
         <v>2000</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="1" t="n">
@@ -590,7 +581,7 @@
       <c r="A12" s="3" t="n">
         <v>2000</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="1" t="n">
@@ -613,7 +604,7 @@
       <c r="A13" s="3" t="n">
         <v>2000</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1" t="n">
@@ -636,7 +627,7 @@
       <c r="A14" s="3" t="n">
         <v>2000</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="n">
@@ -659,7 +650,7 @@
       <c r="A15" s="3" t="n">
         <v>2001</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="1" t="n">
@@ -682,7 +673,7 @@
       <c r="A16" s="3" t="n">
         <v>2001</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="1" t="n">
@@ -705,7 +696,7 @@
       <c r="A17" s="3" t="n">
         <v>2001</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="1" t="n">
@@ -728,7 +719,7 @@
       <c r="A18" s="3" t="n">
         <v>2001</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="1" t="n">
@@ -751,7 +742,7 @@
       <c r="A19" s="3" t="n">
         <v>2002</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="1" t="n">
@@ -774,7 +765,7 @@
       <c r="A20" s="3" t="n">
         <v>2002</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="n">
@@ -797,7 +788,7 @@
       <c r="A21" s="3" t="n">
         <v>2002</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="1" t="n">
@@ -820,7 +811,7 @@
       <c r="A22" s="3" t="n">
         <v>2002</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="n">
@@ -843,7 +834,7 @@
       <c r="A23" s="3" t="n">
         <v>2003</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C23" s="1" t="n">
@@ -866,7 +857,7 @@
       <c r="A24" s="3" t="n">
         <v>2003</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C24" s="1" t="n">
@@ -889,7 +880,7 @@
       <c r="A25" s="3" t="n">
         <v>2003</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="1" t="n">
@@ -912,7 +903,7 @@
       <c r="A26" s="3" t="n">
         <v>2003</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C26" s="1" t="n">
@@ -935,7 +926,7 @@
       <c r="A27" s="3" t="n">
         <v>2004</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C27" s="1" t="n">
@@ -958,7 +949,7 @@
       <c r="A28" s="3" t="n">
         <v>2004</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="1" t="n">
@@ -981,7 +972,7 @@
       <c r="A29" s="3" t="n">
         <v>2004</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="1" t="n">
@@ -1004,7 +995,7 @@
       <c r="A30" s="3" t="n">
         <v>2004</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="1" t="n">
@@ -1027,7 +1018,7 @@
       <c r="A31" s="3" t="n">
         <v>2005</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C31" s="1" t="n">
@@ -1050,7 +1041,7 @@
       <c r="A32" s="3" t="n">
         <v>2005</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="1" t="n">
@@ -1073,7 +1064,7 @@
       <c r="A33" s="3" t="n">
         <v>2005</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="1" t="n">
@@ -1096,7 +1087,7 @@
       <c r="A34" s="3" t="n">
         <v>2005</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C34" s="1" t="n">
@@ -1119,7 +1110,7 @@
       <c r="A35" s="3" t="n">
         <v>2006</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C35" s="1" t="n">
@@ -1142,7 +1133,7 @@
       <c r="A36" s="3" t="n">
         <v>2006</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C36" s="1" t="n">
@@ -1165,7 +1156,7 @@
       <c r="A37" s="3" t="n">
         <v>2006</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="1" t="n">
@@ -1188,7 +1179,7 @@
       <c r="A38" s="3" t="n">
         <v>2006</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C38" s="1" t="n">
@@ -1211,7 +1202,7 @@
       <c r="A39" s="3" t="n">
         <v>2006</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C39" s="1" t="n">
@@ -1234,7 +1225,7 @@
       <c r="A40" s="3" t="n">
         <v>2007</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C40" s="1" t="n">
@@ -1257,7 +1248,7 @@
       <c r="A41" s="3" t="n">
         <v>2007</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C41" s="1" t="n">
@@ -1280,7 +1271,7 @@
       <c r="A42" s="3" t="n">
         <v>2007</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C42" s="1" t="n">
@@ -1303,7 +1294,7 @@
       <c r="A43" s="3" t="n">
         <v>2007</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="1" t="n">
@@ -1326,7 +1317,7 @@
       <c r="A44" s="3" t="n">
         <v>2007</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C44" s="1" t="n">
@@ -1349,7 +1340,7 @@
       <c r="A45" s="3" t="n">
         <v>2008</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="1" t="n">
@@ -1372,7 +1363,7 @@
       <c r="A46" s="3" t="n">
         <v>2008</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C46" s="1" t="n">
@@ -1395,7 +1386,7 @@
       <c r="A47" s="3" t="n">
         <v>2008</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C47" s="1" t="n">
@@ -1418,7 +1409,7 @@
       <c r="A48" s="3" t="n">
         <v>2008</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C48" s="1" t="n">
@@ -1441,7 +1432,7 @@
       <c r="A49" s="3" t="n">
         <v>2008</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="1" t="n">
@@ -1464,7 +1455,7 @@
       <c r="A50" s="3" t="n">
         <v>2009</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C50" s="1" t="n">
@@ -1487,7 +1478,7 @@
       <c r="A51" s="3" t="n">
         <v>2009</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="1" t="n">
@@ -1510,7 +1501,7 @@
       <c r="A52" s="3" t="n">
         <v>2009</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="1" t="n">
@@ -1533,7 +1524,7 @@
       <c r="A53" s="3" t="n">
         <v>2009</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C53" s="1" t="n">
@@ -1556,7 +1547,7 @@
       <c r="A54" s="3" t="n">
         <v>2009</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C54" s="1" t="n">
@@ -1579,7 +1570,7 @@
       <c r="A55" s="3" t="n">
         <v>2010</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C55" s="1" t="n">
@@ -1602,7 +1593,7 @@
       <c r="A56" s="3" t="n">
         <v>2010</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C56" s="1" t="n">
@@ -1625,7 +1616,7 @@
       <c r="A57" s="3" t="n">
         <v>2010</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C57" s="1" t="n">
@@ -1648,7 +1639,7 @@
       <c r="A58" s="3" t="n">
         <v>2010</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="1" t="n">
@@ -1671,7 +1662,7 @@
       <c r="A59" s="3" t="n">
         <v>2010</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C59" s="1" t="n">
@@ -1694,7 +1685,7 @@
       <c r="A60" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C60" s="1" t="n">
@@ -1717,7 +1708,7 @@
       <c r="A61" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C61" s="1" t="n">
@@ -1740,7 +1731,7 @@
       <c r="A62" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="1" t="n">
@@ -1763,7 +1754,7 @@
       <c r="A63" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C63" s="1" t="n">
@@ -1786,7 +1777,7 @@
       <c r="A64" s="3" t="n">
         <v>2011</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C64" s="1" t="n">
@@ -1809,7 +1800,7 @@
       <c r="A65" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C65" s="1" t="n">
@@ -1832,7 +1823,7 @@
       <c r="A66" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C66" s="1" t="n">
@@ -1855,7 +1846,7 @@
       <c r="A67" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B67" s="4" t="s">
+      <c r="B67" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C67" s="1" t="n">
@@ -1878,7 +1869,7 @@
       <c r="A68" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B68" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="1" t="n">
@@ -1901,7 +1892,7 @@
       <c r="A69" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C69" s="1" t="n">
@@ -1924,7 +1915,7 @@
       <c r="A70" s="3" t="n">
         <v>2012</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B70" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C70" s="1" t="n">
@@ -1947,7 +1938,7 @@
       <c r="A71" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C71" s="1" t="n">
@@ -1970,7 +1961,7 @@
       <c r="A72" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="B72" s="4" t="s">
+      <c r="B72" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C72" s="1" t="n">
@@ -1993,7 +1984,7 @@
       <c r="A73" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="B73" s="4" t="s">
+      <c r="B73" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C73" s="1" t="n">
@@ -2016,7 +2007,7 @@
       <c r="A74" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C74" s="1" t="n">
@@ -2039,7 +2030,7 @@
       <c r="A75" s="3" t="n">
         <v>2013</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C75" s="1" t="n">
@@ -2062,7 +2053,7 @@
       <c r="A76" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B76" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C76" s="1" t="n">
@@ -2085,7 +2076,7 @@
       <c r="A77" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B77" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C77" s="1" t="n">
@@ -2108,7 +2099,7 @@
       <c r="A78" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B78" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C78" s="1" t="n">
@@ -2131,7 +2122,7 @@
       <c r="A79" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="1" t="n">
@@ -2154,7 +2145,7 @@
       <c r="A80" s="3" t="n">
         <v>2014</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B80" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C80" s="1" t="n">
@@ -2177,7 +2168,7 @@
       <c r="A81" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C81" s="1" t="n">
@@ -2200,7 +2191,7 @@
       <c r="A82" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B82" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C82" s="1" t="n">
@@ -2223,7 +2214,7 @@
       <c r="A83" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B83" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C83" s="1" t="n">
@@ -2246,7 +2237,7 @@
       <c r="A84" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C84" s="1" t="n">
@@ -2269,7 +2260,7 @@
       <c r="A85" s="3" t="n">
         <v>2015</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C85" s="1" t="n">
@@ -2292,7 +2283,7 @@
       <c r="A86" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C86" s="1" t="n">
@@ -2315,7 +2306,7 @@
       <c r="A87" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C87" s="1" t="n">
@@ -2338,7 +2329,7 @@
       <c r="A88" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="B88" s="4" t="s">
+      <c r="B88" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C88" s="1" t="n">
@@ -2361,7 +2352,7 @@
       <c r="A89" s="3" t="n">
         <v>2016</v>
       </c>
-      <c r="B89" s="4" t="s">
+      <c r="B89" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C89" s="1" t="n">
@@ -2384,7 +2375,7 @@
       <c r="A90" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="B90" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C90" s="1" t="n">
@@ -2399,7 +2390,7 @@
       <c r="F90" s="1" t="n">
         <v>546.916211648571</v>
       </c>
-      <c r="G90" s="5" t="n">
+      <c r="G90" s="4" t="n">
         <v>537.985714285715</v>
       </c>
     </row>
@@ -2407,7 +2398,7 @@
       <c r="A91" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="B91" s="4" t="s">
+      <c r="B91" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C91" s="1" t="n">
@@ -2430,7 +2421,7 @@
       <c r="A92" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="B92" s="4" t="s">
+      <c r="B92" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="1" t="n">
@@ -2453,7 +2444,7 @@
       <c r="A93" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="B93" s="4" t="s">
+      <c r="B93" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C93" s="1" t="n">
@@ -2476,7 +2467,7 @@
       <c r="A94" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="B94" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C94" s="1" t="n">
@@ -2499,7 +2490,7 @@
       <c r="A95" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C95" s="1" t="n">
@@ -2522,7 +2513,7 @@
       <c r="A96" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B96" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C96" s="1" t="n">
@@ -2545,7 +2536,7 @@
       <c r="A97" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B97" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C97" s="1" t="n">
@@ -2568,7 +2559,7 @@
       <c r="A98" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B98" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="1" t="n">
@@ -2591,7 +2582,7 @@
       <c r="A99" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C99" s="1" t="n">
@@ -2614,7 +2605,7 @@
       <c r="A100" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C100" s="1" t="n">
@@ -2637,7 +2628,7 @@
       <c r="A101" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B101" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C101" s="1" t="n">
@@ -2660,7 +2651,7 @@
       <c r="A102" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B102" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C102" s="1" t="n">
@@ -2683,7 +2674,7 @@
       <c r="A103" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B103" s="4" t="s">
+      <c r="B103" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C103" s="1" t="n">
@@ -2706,7 +2697,7 @@
       <c r="A104" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B104" s="4" t="s">
+      <c r="B104" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C104" s="1" t="n">
@@ -2729,7 +2720,7 @@
       <c r="A105" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B105" s="4" t="s">
+      <c r="B105" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C105" s="1" t="n">
@@ -2752,7 +2743,7 @@
       <c r="A106" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B106" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C106" s="1" t="n">
@@ -2775,7 +2766,7 @@
       <c r="A107" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="B107" s="4" t="s">
+      <c r="B107" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C107" s="1" t="n">
@@ -2798,7 +2789,7 @@
       <c r="A108" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="B108" s="4" t="s">
+      <c r="B108" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C108" s="1" t="n">
@@ -2821,7 +2812,7 @@
       <c r="A109" s="3" t="n">
         <v>2021</v>
       </c>
-      <c r="B109" s="4" t="s">
+      <c r="B109" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C109" s="1" t="n">
@@ -2844,7 +2835,7 @@
       <c r="A110" s="3" t="n">
         <v>2022</v>
       </c>
-      <c r="B110" s="4" t="s">
+      <c r="B110" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C110" s="1" t="n">
@@ -2867,7 +2858,7 @@
       <c r="A111" s="3" t="n">
         <v>2022</v>
       </c>
-      <c r="B111" s="4" t="s">
+      <c r="B111" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C111" s="1" t="n">
@@ -2890,7 +2881,7 @@
       <c r="A112" s="3" t="n">
         <v>2022</v>
       </c>
-      <c r="B112" s="4" t="s">
+      <c r="B112" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C112" s="1" t="n">
@@ -2913,7 +2904,7 @@
       <c r="A113" s="3" t="n">
         <v>2022</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B113" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C113" s="1" t="n">
@@ -2936,7 +2927,7 @@
       <c r="A114" s="3" t="n">
         <v>2023</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B114" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C114" s="1" t="n">
@@ -2959,7 +2950,7 @@
       <c r="A115" s="3" t="n">
         <v>2023</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B115" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C115" s="1" t="n">
@@ -2982,7 +2973,7 @@
       <c r="A116" s="3" t="n">
         <v>2023</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B116" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C116" s="1" t="n">
@@ -3005,7 +2996,7 @@
       <c r="A117" s="3" t="n">
         <v>2023</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B117" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C117" s="1" t="n">
@@ -3028,7 +3019,7 @@
       <c r="A118" s="3" t="n">
         <v>2024</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B118" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C118" s="1" t="n">
@@ -3051,7 +3042,7 @@
       <c r="A119" s="3" t="n">
         <v>2024</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B119" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C119" s="1" t="n">
@@ -3074,7 +3065,7 @@
       <c r="A120" s="3" t="n">
         <v>2024</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B120" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C120" s="1" t="n">
@@ -3097,7 +3088,7 @@
       <c r="A121" s="3" t="n">
         <v>2024</v>
       </c>
-      <c r="B121" s="4" t="s">
+      <c r="B121" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C121" s="1" t="n">
@@ -3120,7 +3111,7 @@
       <c r="A122" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="B122" s="4" t="s">
+      <c r="B122" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C122" s="1" t="n">
@@ -3143,7 +3134,7 @@
       <c r="A123" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="B123" s="4" t="s">
+      <c r="B123" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C123" s="1" t="n">
@@ -3166,7 +3157,7 @@
       <c r="A124" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="B124" s="4" t="s">
+      <c r="B124" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C124" s="1" t="n">
@@ -3189,7 +3180,7 @@
       <c r="A125" s="3" t="n">
         <v>2025</v>
       </c>
-      <c r="B125" s="4" t="s">
+      <c r="B125" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C125" s="1" t="n">
@@ -3212,7 +3203,7 @@
       <c r="A126" s="3" t="n">
         <v>2026</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C126" s="1" t="n">
@@ -3235,7 +3226,7 @@
       <c r="A127" s="3" t="n">
         <v>2026</v>
       </c>
-      <c r="B127" s="4" t="s">
+      <c r="B127" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C127" s="1" t="n">
@@ -3258,7 +3249,7 @@
       <c r="A128" s="3" t="n">
         <v>2026</v>
       </c>
-      <c r="B128" s="4" t="s">
+      <c r="B128" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C128" s="1" t="n">
@@ -3281,7 +3272,7 @@
       <c r="A129" s="3" t="n">
         <v>2026</v>
       </c>
-      <c r="B129" s="4" t="s">
+      <c r="B129" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C129" s="1" t="n">
@@ -3304,7 +3295,7 @@
       <c r="A130" s="3" t="n">
         <v>2027</v>
       </c>
-      <c r="B130" s="4" t="s">
+      <c r="B130" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C130" s="1" t="n">
@@ -3327,7 +3318,7 @@
       <c r="A131" s="3" t="n">
         <v>2027</v>
       </c>
-      <c r="B131" s="4" t="s">
+      <c r="B131" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C131" s="1" t="n">
@@ -3350,7 +3341,7 @@
       <c r="A132" s="3" t="n">
         <v>2027</v>
       </c>
-      <c r="B132" s="4" t="s">
+      <c r="B132" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C132" s="1" t="n">
@@ -3373,7 +3364,7 @@
       <c r="A133" s="3" t="n">
         <v>2027</v>
       </c>
-      <c r="B133" s="4" t="s">
+      <c r="B133" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C133" s="1" t="n">
@@ -3396,7 +3387,7 @@
       <c r="A134" s="3" t="n">
         <v>2028</v>
       </c>
-      <c r="B134" s="4" t="s">
+      <c r="B134" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C134" s="1" t="n">
@@ -3419,7 +3410,7 @@
       <c r="A135" s="3" t="n">
         <v>2028</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C135" s="1" t="n">
@@ -3442,7 +3433,7 @@
       <c r="A136" s="3" t="n">
         <v>2028</v>
       </c>
-      <c r="B136" s="4" t="s">
+      <c r="B136" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C136" s="1" t="n">
@@ -3465,7 +3456,7 @@
       <c r="A137" s="3" t="n">
         <v>2028</v>
       </c>
-      <c r="B137" s="4" t="s">
+      <c r="B137" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C137" s="1" t="n">
@@ -3488,7 +3479,7 @@
       <c r="A138" s="3" t="n">
         <v>2029</v>
       </c>
-      <c r="B138" s="4" t="s">
+      <c r="B138" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C138" s="1" t="n">
@@ -3511,7 +3502,7 @@
       <c r="A139" s="3" t="n">
         <v>2029</v>
       </c>
-      <c r="B139" s="4" t="s">
+      <c r="B139" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C139" s="1" t="n">
@@ -3534,7 +3525,7 @@
       <c r="A140" s="3" t="n">
         <v>2029</v>
       </c>
-      <c r="B140" s="4" t="s">
+      <c r="B140" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C140" s="1" t="n">
@@ -3557,7 +3548,7 @@
       <c r="A141" s="3" t="n">
         <v>2029</v>
       </c>
-      <c r="B141" s="4" t="s">
+      <c r="B141" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C141" s="1" t="n">
@@ -3580,7 +3571,7 @@
       <c r="A142" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="B142" s="4" t="s">
+      <c r="B142" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C142" s="1" t="n">
@@ -3603,7 +3594,7 @@
       <c r="A143" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="B143" s="4" t="s">
+      <c r="B143" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C143" s="1" t="n">
@@ -3626,7 +3617,7 @@
       <c r="A144" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="B144" s="4" t="s">
+      <c r="B144" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C144" s="1" t="n">
@@ -3649,7 +3640,7 @@
       <c r="A145" s="3" t="n">
         <v>2030</v>
       </c>
-      <c r="B145" s="4" t="s">
+      <c r="B145" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C145" s="1" t="n">
@@ -3672,92 +3663,92 @@
       <c r="A146" s="3" t="n">
         <v>2031</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B146" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C146" s="2" t="n">
-        <v>474.617592534601</v>
-      </c>
-      <c r="D146" s="2" t="n">
-        <v>447.941246776269</v>
-      </c>
-      <c r="E146" s="2" t="n">
-        <v>510.335970902953</v>
-      </c>
-      <c r="F146" s="2" t="n">
-        <v>478.708009894287</v>
-      </c>
-      <c r="G146" s="2" t="n">
-        <v>480.248857142858</v>
+      <c r="C146" s="0" t="n">
+        <v>450.580567555001</v>
+      </c>
+      <c r="D146" s="0" t="n">
+        <v>402.374271113335</v>
+      </c>
+      <c r="E146" s="0" t="n">
+        <v>487.782542911905</v>
+      </c>
+      <c r="F146" s="0" t="n">
+        <v>385.611064928571</v>
+      </c>
+      <c r="G146" s="0" t="n">
+        <v>433.435714285716</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="3" t="n">
         <v>2031</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B147" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>499.440217051277</v>
+        <v>474.416999538349</v>
       </c>
       <c r="D147" s="0" t="n">
-        <v>472.436892461708</v>
+        <v>425.199080633104</v>
       </c>
       <c r="E147" s="0" t="n">
-        <v>570.6750988446</v>
+        <v>545.82658149095</v>
       </c>
       <c r="F147" s="0" t="n">
-        <v>524.129354506547</v>
+        <v>426.010320429421</v>
       </c>
       <c r="G147" s="0" t="n">
-        <v>494.975791832107</v>
+        <v>447.218288459103</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="3" t="n">
         <v>2031</v>
       </c>
-      <c r="B148" s="4" t="s">
+      <c r="B148" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>449.794968017926</v>
+        <v>426.744135571652</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>423.44560109083</v>
+        <v>379.549461593566</v>
       </c>
       <c r="E148" s="0" t="n">
-        <v>449.996842961306</v>
+        <v>429.73850433286</v>
       </c>
       <c r="F148" s="0" t="n">
-        <v>433.286665282026</v>
+        <v>345.211809427724</v>
       </c>
       <c r="G148" s="0" t="n">
-        <v>465.521922453609</v>
+        <v>419.653140112327</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="3" t="n">
         <v>2031</v>
       </c>
-      <c r="B149" s="4" t="s">
+      <c r="B149" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>464.050959580001</v>
+        <v>450.580567555001</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>420.607849493335</v>
+        <v>402.374271113335</v>
       </c>
       <c r="E149" s="0" t="n">
-        <v>499.474624930476</v>
+        <v>487.782542911906</v>
       </c>
       <c r="F149" s="0" t="n">
-        <v>408.654657317143</v>
+        <v>385.611064928573</v>
       </c>
       <c r="G149" s="0" t="n">
-        <v>448.371428571429</v>
+        <v>433.435714285715</v>
       </c>
     </row>
   </sheetData>
@@ -3779,106 +3770,106 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="C146:G149 B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="120.188775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="118.790816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="7" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>